<commit_message>
add new Panama species list, revise code to check it, and revised temp check files
</commit_message>
<xml_diff>
--- a/tocheck/tempdupbinomial.xlsx
+++ b/tocheck/tempdupbinomial.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -385,121 +385,37 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Subspecies</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Synonyms</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Herbarium</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Spcode</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Liana</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>binomial</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Fabales</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Fabaceae</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Swartzia</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>simplex</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>(Sw.) Spreng.</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Swartzia simplex var. grandiflora</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>R. Pérez 2188 (PMA, SCZ)</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>swars1</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Swartzia simplex</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Fabales</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Fabaceae</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Swartzia</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>simplex</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>(Sw.) Spreng.</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Swartzia simplex var. continentalis</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>R. Pérez 1973 y 2021 (PMA, SCZ)</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>swars2</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Swartzia simplex</t>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>fullname</t>
         </is>
       </c>
     </row>

</xml_diff>